<commit_message>
updates to support bad files and additional access levels
</commit_message>
<xml_diff>
--- a/seed/tests/data/access-level-instances.xlsx
+++ b/seed/tests/data/access-level-instances.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kflemin/repos/seed/seed/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kflemin/repos/seed-TESTING/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AFEF4D-47B1-EB4C-A9C1-FCAE49405B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F08955-601A-2145-82FD-3514A62CB5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11820" yWindow="500" windowWidth="23460" windowHeight="18900" xr2:uid="{4148A922-1273-D04B-A5DE-CD2D27F49048}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>Utility</t>
   </si>
   <si>
-    <t>Organization</t>
-  </si>
-  <si>
     <t>Data Center A</t>
   </si>
   <si>
@@ -291,6 +288,9 @@
   </si>
   <si>
     <t>Sub Sector</t>
+  </si>
+  <si>
+    <t>Partner</t>
   </si>
 </sst>
 </file>
@@ -665,10 +665,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -679,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -712,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -767,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -778,7 +778,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -789,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -800,7 +800,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -811,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -822,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -833,7 +833,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -844,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -855,7 +855,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -866,7 +866,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -877,7 +877,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -888,7 +888,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -899,7 +899,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -910,7 +910,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -921,7 +921,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -932,7 +932,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -943,7 +943,7 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -954,7 +954,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -965,7 +965,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -976,7 +976,7 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -987,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -998,7 +998,7 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,7 +1020,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1031,7 +1031,7 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1053,7 +1053,7 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1064,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1075,7 +1075,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1086,7 +1086,7 @@
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1097,7 +1097,7 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1108,7 +1108,7 @@
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1119,7 +1119,7 @@
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1130,7 +1130,7 @@
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1141,7 +1141,7 @@
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1152,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1163,7 +1163,7 @@
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1185,7 +1185,7 @@
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1207,7 +1207,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1229,7 +1229,7 @@
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1240,7 +1240,7 @@
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1251,7 +1251,7 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1262,7 +1262,7 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1273,7 +1273,7 @@
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1284,7 +1284,7 @@
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1328,7 +1328,7 @@
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1339,7 +1339,7 @@
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1372,7 +1372,7 @@
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1383,7 +1383,7 @@
         <v>10</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1394,7 +1394,7 @@
         <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1405,7 +1405,7 @@
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1416,7 +1416,7 @@
         <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1427,7 +1427,7 @@
         <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1438,7 +1438,7 @@
         <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1449,7 +1449,7 @@
         <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>